<commit_message>
refactor: Update Actions component to use more descriptive prop names
</commit_message>
<xml_diff>
--- a/public/cek-tarif.xlsx
+++ b/public/cek-tarif.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">HS CODE</t>
   </si>
@@ -29,15 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">49111090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85365099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39191099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82130000</t>
   </si>
 </sst>
 </file>
@@ -142,10 +133,10 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -166,43 +157,29 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+    </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>